<commit_message>
I kept the mapping for Current Claim Unique ID as in the original, but surfaced the note about the mapping not being 1:1 in each relevant field in the spreadsheet
</commit_message>
<xml_diff>
--- a/assets/data/CCLF_BCDA_BB_Crosswalk.xlsx
+++ b/assets/data/CCLF_BCDA_BB_Crosswalk.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesmcconnell/bcda-static-site/assets/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9BA9652-40CA-1448-84AD-4C2D3C814B8C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCA54984-E92D-9949-8AF1-330E65626E49}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39300" yWindow="1500" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="1500" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All CCLF Files" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2437" uniqueCount="856">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2445" uniqueCount="856">
   <si>
     <t>CCLF Claim Field Label</t>
   </si>
@@ -3188,7 +3188,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3219,6 +3219,12 @@
         <bgColor rgb="FF5B95F9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE8F0FE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -3232,7 +3238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -3338,6 +3344,12 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3580,6 +3592,11 @@
       <tableStyleElement type="secondRowStripe" dxfId="0"/>
     </tableStyle>
   </tableStyles>
+  <colors>
+    <mruColors>
+      <color rgb="FFE8F0FE"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -3891,13 +3908,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:R237"/>
+  <dimension ref="A1:R990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B227" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B195" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E990" sqref="E990"/>
+      <selection pane="bottomRight" activeCell="E198" sqref="E198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -3969,7 +3986,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="174">
+    <row r="2" spans="1:18" ht="43">
       <c r="A2" s="5" t="s">
         <v>14</v>
       </c>
@@ -3988,7 +4005,9 @@
       <c r="F2" s="15" t="s">
         <v>683</v>
       </c>
-      <c r="G2" s="16"/>
+      <c r="G2" s="5" t="s">
+        <v>684</v>
+      </c>
       <c r="H2" s="2" t="s">
         <v>39</v>
       </c>
@@ -4016,9 +4035,7 @@
       <c r="P2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="Q2" s="5" t="s">
-        <v>684</v>
-      </c>
+      <c r="Q2" s="5"/>
       <c r="R2" s="2" t="s">
         <v>685</v>
       </c>
@@ -4511,7 +4528,7 @@
       <c r="E12" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="F12" s="21" t="s">
+      <c r="F12" s="38" t="s">
         <v>701</v>
       </c>
       <c r="G12" s="16"/>
@@ -5865,7 +5882,7 @@
       <c r="Q39" s="12"/>
       <c r="R39" s="25"/>
     </row>
-    <row r="40" spans="1:18" ht="30">
+    <row r="40" spans="1:18" ht="43">
       <c r="A40" s="5" t="s">
         <v>14</v>
       </c>
@@ -5884,7 +5901,9 @@
       <c r="F40" s="15" t="s">
         <v>683</v>
       </c>
-      <c r="G40" s="16"/>
+      <c r="G40" s="5" t="s">
+        <v>684</v>
+      </c>
       <c r="H40" s="2" t="s">
         <v>304</v>
       </c>
@@ -7000,7 +7019,9 @@
       <c r="F63" s="18" t="s">
         <v>751</v>
       </c>
-      <c r="G63" s="19"/>
+      <c r="G63" s="5" t="s">
+        <v>684</v>
+      </c>
       <c r="H63" s="1" t="s">
         <v>449</v>
       </c>
@@ -7241,7 +7262,7 @@
       <c r="E68" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="F68" s="21" t="s">
+      <c r="F68" s="38" t="s">
         <v>754</v>
       </c>
       <c r="G68" s="16"/>
@@ -7591,7 +7612,7 @@
       <c r="Q75" s="12"/>
       <c r="R75" s="25"/>
     </row>
-    <row r="76" spans="1:18" ht="30">
+    <row r="76" spans="1:18" ht="43">
       <c r="A76" s="5" t="s">
         <v>14</v>
       </c>
@@ -7610,7 +7631,9 @@
       <c r="F76" s="15" t="s">
         <v>683</v>
       </c>
-      <c r="G76" s="16"/>
+      <c r="G76" s="5" t="s">
+        <v>684</v>
+      </c>
       <c r="H76" s="2" t="s">
         <v>466</v>
       </c>
@@ -7809,7 +7832,7 @@
       <c r="E80" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="F80" s="21" t="s">
+      <c r="F80" s="38" t="s">
         <v>757</v>
       </c>
       <c r="G80" s="16"/>
@@ -7903,7 +7926,7 @@
       <c r="E82" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="F82" s="21" t="s">
+      <c r="F82" s="38" t="s">
         <v>760</v>
       </c>
       <c r="G82" s="16"/>
@@ -8257,7 +8280,7 @@
       <c r="Q89" s="12"/>
       <c r="R89" s="25"/>
     </row>
-    <row r="90" spans="1:18" ht="30">
+    <row r="90" spans="1:18" ht="43">
       <c r="A90" s="5" t="s">
         <v>14</v>
       </c>
@@ -8276,7 +8299,9 @@
       <c r="F90" s="15" t="s">
         <v>683</v>
       </c>
-      <c r="G90" s="16"/>
+      <c r="G90" s="5" t="s">
+        <v>684</v>
+      </c>
       <c r="H90" s="2" t="s">
         <v>539</v>
       </c>
@@ -10729,7 +10754,7 @@
       <c r="Q139" s="12"/>
       <c r="R139" s="25"/>
     </row>
-    <row r="140" spans="1:18" ht="30">
+    <row r="140" spans="1:18" ht="43">
       <c r="A140" s="5" t="s">
         <v>14</v>
       </c>
@@ -10748,7 +10773,9 @@
       <c r="F140" s="15" t="s">
         <v>683</v>
       </c>
-      <c r="G140" s="16"/>
+      <c r="G140" s="5" t="s">
+        <v>684</v>
+      </c>
       <c r="H140" s="2" t="s">
         <v>658</v>
       </c>
@@ -12008,7 +12035,7 @@
       <c r="Q165" s="12"/>
       <c r="R165" s="25"/>
     </row>
-    <row r="166" spans="1:18" ht="30">
+    <row r="166" spans="1:18" ht="43">
       <c r="A166" s="5" t="s">
         <v>14</v>
       </c>
@@ -12027,7 +12054,9 @@
       <c r="F166" s="15" t="s">
         <v>810</v>
       </c>
-      <c r="G166" s="16"/>
+      <c r="G166" s="5" t="s">
+        <v>684</v>
+      </c>
       <c r="H166" s="2" t="s">
         <v>662</v>
       </c>
@@ -12632,7 +12661,7 @@
       <c r="E178" s="2" t="s">
         <v>508</v>
       </c>
-      <c r="F178" s="21" t="s">
+      <c r="F178" s="38" t="s">
         <v>821</v>
       </c>
       <c r="G178" s="16" t="s">
@@ -12736,7 +12765,7 @@
       <c r="E180" s="2" t="s">
         <v>519</v>
       </c>
-      <c r="F180" s="21" t="s">
+      <c r="F180" s="38" t="s">
         <v>824</v>
       </c>
       <c r="G180" s="16"/>
@@ -13564,7 +13593,7 @@
       <c r="E198" s="2" t="s">
         <v>569</v>
       </c>
-      <c r="F198" s="21" t="s">
+      <c r="F198" s="38" t="s">
         <v>839</v>
       </c>
       <c r="G198" s="16"/>
@@ -14846,7 +14875,7 @@
       <c r="Q226" s="12"/>
       <c r="R226" s="25"/>
     </row>
-    <row r="227" spans="1:18" ht="30">
+    <row r="227" spans="1:18" ht="43">
       <c r="A227" s="4" t="s">
         <v>14</v>
       </c>
@@ -14861,7 +14890,9 @@
       <c r="F227" s="18" t="s">
         <v>683</v>
       </c>
-      <c r="G227" s="19"/>
+      <c r="G227" s="5" t="s">
+        <v>684</v>
+      </c>
       <c r="H227" s="11" t="s">
         <v>671</v>
       </c>
@@ -15102,7 +15133,7 @@
       <c r="Q232" s="12"/>
       <c r="R232" s="25"/>
     </row>
-    <row r="233" spans="1:18" ht="30">
+    <row r="233" spans="1:18" ht="43">
       <c r="A233" s="4" t="s">
         <v>14</v>
       </c>
@@ -15117,7 +15148,9 @@
       <c r="F233" s="18" t="s">
         <v>683</v>
       </c>
-      <c r="G233" s="19"/>
+      <c r="G233" s="5" t="s">
+        <v>684</v>
+      </c>
       <c r="H233" s="11" t="s">
         <v>678</v>
       </c>
@@ -15337,6 +15370,2265 @@
       <c r="R237" s="1" t="s">
         <v>692</v>
       </c>
+    </row>
+    <row r="238" spans="1:18" ht="15.75" customHeight="1">
+      <c r="G238" s="19"/>
+    </row>
+    <row r="239" spans="1:18" ht="15.75" customHeight="1">
+      <c r="G239" s="16"/>
+    </row>
+    <row r="240" spans="1:18" ht="15.75" customHeight="1">
+      <c r="G240" s="19"/>
+    </row>
+    <row r="241" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G241" s="16"/>
+    </row>
+    <row r="242" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G242" s="19"/>
+    </row>
+    <row r="243" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G243" s="16"/>
+    </row>
+    <row r="244" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G244" s="19"/>
+    </row>
+    <row r="245" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G245" s="16"/>
+    </row>
+    <row r="246" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G246" s="19"/>
+    </row>
+    <row r="247" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G247" s="16"/>
+    </row>
+    <row r="248" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G248" s="19"/>
+    </row>
+    <row r="249" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G249" s="16"/>
+    </row>
+    <row r="250" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G250" s="19"/>
+    </row>
+    <row r="251" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G251" s="16"/>
+    </row>
+    <row r="252" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G252" s="19"/>
+    </row>
+    <row r="253" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G253" s="16"/>
+    </row>
+    <row r="254" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G254" s="19"/>
+    </row>
+    <row r="255" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G255" s="16"/>
+    </row>
+    <row r="256" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G256" s="19"/>
+    </row>
+    <row r="257" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G257" s="16"/>
+    </row>
+    <row r="258" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G258" s="19"/>
+    </row>
+    <row r="259" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G259" s="16"/>
+    </row>
+    <row r="260" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G260" s="19"/>
+    </row>
+    <row r="261" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G261" s="16"/>
+    </row>
+    <row r="262" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G262" s="19"/>
+    </row>
+    <row r="263" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G263" s="16"/>
+    </row>
+    <row r="264" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G264" s="19"/>
+    </row>
+    <row r="265" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G265" s="16"/>
+    </row>
+    <row r="266" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G266" s="19"/>
+    </row>
+    <row r="267" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G267" s="16"/>
+    </row>
+    <row r="268" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G268" s="19"/>
+    </row>
+    <row r="269" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G269" s="16"/>
+    </row>
+    <row r="270" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G270" s="19"/>
+    </row>
+    <row r="271" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G271" s="16"/>
+    </row>
+    <row r="272" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G272" s="19"/>
+    </row>
+    <row r="273" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G273" s="16"/>
+    </row>
+    <row r="274" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G274" s="19"/>
+    </row>
+    <row r="275" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G275" s="16"/>
+    </row>
+    <row r="276" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G276" s="19"/>
+    </row>
+    <row r="277" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G277" s="16"/>
+    </row>
+    <row r="278" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G278" s="19"/>
+    </row>
+    <row r="279" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G279" s="16"/>
+    </row>
+    <row r="280" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G280" s="19"/>
+    </row>
+    <row r="281" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G281" s="16"/>
+    </row>
+    <row r="282" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G282" s="19"/>
+    </row>
+    <row r="283" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G283" s="16"/>
+    </row>
+    <row r="284" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G284" s="19"/>
+    </row>
+    <row r="285" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G285" s="16"/>
+    </row>
+    <row r="286" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G286" s="19"/>
+    </row>
+    <row r="287" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G287" s="16"/>
+    </row>
+    <row r="288" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G288" s="19"/>
+    </row>
+    <row r="289" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G289" s="16"/>
+    </row>
+    <row r="290" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G290" s="19"/>
+    </row>
+    <row r="291" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G291" s="16"/>
+    </row>
+    <row r="292" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G292" s="19"/>
+    </row>
+    <row r="293" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G293" s="16"/>
+    </row>
+    <row r="294" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G294" s="19"/>
+    </row>
+    <row r="295" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G295" s="16"/>
+    </row>
+    <row r="296" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G296" s="19"/>
+    </row>
+    <row r="297" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G297" s="16"/>
+    </row>
+    <row r="298" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G298" s="19"/>
+    </row>
+    <row r="299" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G299" s="16"/>
+    </row>
+    <row r="300" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G300" s="19"/>
+    </row>
+    <row r="301" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G301" s="16"/>
+    </row>
+    <row r="302" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G302" s="19"/>
+    </row>
+    <row r="303" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G303" s="16"/>
+    </row>
+    <row r="304" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G304" s="19"/>
+    </row>
+    <row r="305" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G305" s="16"/>
+    </row>
+    <row r="306" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G306" s="19"/>
+    </row>
+    <row r="307" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G307" s="16"/>
+    </row>
+    <row r="308" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G308" s="19"/>
+    </row>
+    <row r="309" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G309" s="16"/>
+    </row>
+    <row r="310" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G310" s="19"/>
+    </row>
+    <row r="311" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G311" s="16"/>
+    </row>
+    <row r="312" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G312" s="19"/>
+    </row>
+    <row r="313" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G313" s="16"/>
+    </row>
+    <row r="314" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G314" s="19"/>
+    </row>
+    <row r="315" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G315" s="16"/>
+    </row>
+    <row r="316" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G316" s="19"/>
+    </row>
+    <row r="317" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G317" s="16"/>
+    </row>
+    <row r="318" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G318" s="19"/>
+    </row>
+    <row r="319" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G319" s="16"/>
+    </row>
+    <row r="320" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G320" s="19"/>
+    </row>
+    <row r="321" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G321" s="16"/>
+    </row>
+    <row r="322" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G322" s="19"/>
+    </row>
+    <row r="323" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G323" s="16"/>
+    </row>
+    <row r="324" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G324" s="19"/>
+    </row>
+    <row r="325" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G325" s="16"/>
+    </row>
+    <row r="326" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G326" s="19"/>
+    </row>
+    <row r="327" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G327" s="16"/>
+    </row>
+    <row r="328" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G328" s="19"/>
+    </row>
+    <row r="329" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G329" s="16"/>
+    </row>
+    <row r="330" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G330" s="19"/>
+    </row>
+    <row r="331" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G331" s="16"/>
+    </row>
+    <row r="332" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G332" s="19"/>
+    </row>
+    <row r="333" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G333" s="16"/>
+    </row>
+    <row r="334" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G334" s="19"/>
+    </row>
+    <row r="335" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G335" s="16"/>
+    </row>
+    <row r="336" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G336" s="19"/>
+    </row>
+    <row r="337" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G337" s="16"/>
+    </row>
+    <row r="338" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G338" s="19"/>
+    </row>
+    <row r="339" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G339" s="16"/>
+    </row>
+    <row r="340" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G340" s="19"/>
+    </row>
+    <row r="341" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G341" s="16"/>
+    </row>
+    <row r="342" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G342" s="19"/>
+    </row>
+    <row r="343" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G343" s="16"/>
+    </row>
+    <row r="344" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G344" s="19"/>
+    </row>
+    <row r="345" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G345" s="16"/>
+    </row>
+    <row r="346" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G346" s="19"/>
+    </row>
+    <row r="347" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G347" s="16"/>
+    </row>
+    <row r="348" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G348" s="19"/>
+    </row>
+    <row r="349" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G349" s="16"/>
+    </row>
+    <row r="350" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G350" s="19"/>
+    </row>
+    <row r="351" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G351" s="16"/>
+    </row>
+    <row r="352" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G352" s="19"/>
+    </row>
+    <row r="353" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G353" s="16"/>
+    </row>
+    <row r="354" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G354" s="19"/>
+    </row>
+    <row r="355" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G355" s="16"/>
+    </row>
+    <row r="356" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G356" s="19"/>
+    </row>
+    <row r="357" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G357" s="16"/>
+    </row>
+    <row r="358" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G358" s="19"/>
+    </row>
+    <row r="359" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G359" s="16"/>
+    </row>
+    <row r="360" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G360" s="19"/>
+    </row>
+    <row r="361" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G361" s="16"/>
+    </row>
+    <row r="362" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G362" s="19"/>
+    </row>
+    <row r="363" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G363" s="16"/>
+    </row>
+    <row r="364" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G364" s="19"/>
+    </row>
+    <row r="365" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G365" s="16"/>
+    </row>
+    <row r="366" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G366" s="19"/>
+    </row>
+    <row r="367" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G367" s="16"/>
+    </row>
+    <row r="368" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G368" s="19"/>
+    </row>
+    <row r="369" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G369" s="16"/>
+    </row>
+    <row r="370" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G370" s="19"/>
+    </row>
+    <row r="371" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G371" s="16"/>
+    </row>
+    <row r="372" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G372" s="19"/>
+    </row>
+    <row r="373" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G373" s="16"/>
+    </row>
+    <row r="374" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G374" s="19"/>
+    </row>
+    <row r="375" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G375" s="16"/>
+    </row>
+    <row r="376" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G376" s="19"/>
+    </row>
+    <row r="377" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G377" s="16"/>
+    </row>
+    <row r="378" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G378" s="19"/>
+    </row>
+    <row r="379" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G379" s="16"/>
+    </row>
+    <row r="380" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G380" s="19"/>
+    </row>
+    <row r="381" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G381" s="16"/>
+    </row>
+    <row r="382" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G382" s="19"/>
+    </row>
+    <row r="383" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G383" s="16"/>
+    </row>
+    <row r="384" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G384" s="19"/>
+    </row>
+    <row r="385" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G385" s="16"/>
+    </row>
+    <row r="386" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G386" s="19"/>
+    </row>
+    <row r="387" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G387" s="16"/>
+    </row>
+    <row r="388" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G388" s="19"/>
+    </row>
+    <row r="389" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G389" s="16"/>
+    </row>
+    <row r="390" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G390" s="19"/>
+    </row>
+    <row r="391" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G391" s="16"/>
+    </row>
+    <row r="392" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G392" s="19"/>
+    </row>
+    <row r="393" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G393" s="16"/>
+    </row>
+    <row r="394" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G394" s="19"/>
+    </row>
+    <row r="395" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G395" s="16"/>
+    </row>
+    <row r="396" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G396" s="19"/>
+    </row>
+    <row r="397" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G397" s="16"/>
+    </row>
+    <row r="398" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G398" s="19"/>
+    </row>
+    <row r="399" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G399" s="16"/>
+    </row>
+    <row r="400" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G400" s="19"/>
+    </row>
+    <row r="401" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G401" s="16"/>
+    </row>
+    <row r="402" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G402" s="19"/>
+    </row>
+    <row r="403" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G403" s="16"/>
+    </row>
+    <row r="404" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G404" s="19"/>
+    </row>
+    <row r="405" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G405" s="16"/>
+    </row>
+    <row r="406" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G406" s="19"/>
+    </row>
+    <row r="407" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G407" s="16"/>
+    </row>
+    <row r="408" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G408" s="19"/>
+    </row>
+    <row r="409" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G409" s="16"/>
+    </row>
+    <row r="410" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G410" s="19"/>
+    </row>
+    <row r="411" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G411" s="16"/>
+    </row>
+    <row r="412" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G412" s="19"/>
+    </row>
+    <row r="413" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G413" s="16"/>
+    </row>
+    <row r="414" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G414" s="19"/>
+    </row>
+    <row r="415" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G415" s="16"/>
+    </row>
+    <row r="416" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G416" s="19"/>
+    </row>
+    <row r="417" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G417" s="16"/>
+    </row>
+    <row r="418" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G418" s="19"/>
+    </row>
+    <row r="419" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G419" s="16"/>
+    </row>
+    <row r="420" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G420" s="19"/>
+    </row>
+    <row r="421" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G421" s="16"/>
+    </row>
+    <row r="422" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G422" s="19"/>
+    </row>
+    <row r="423" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G423" s="16"/>
+    </row>
+    <row r="424" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G424" s="19"/>
+    </row>
+    <row r="425" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G425" s="16"/>
+    </row>
+    <row r="426" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G426" s="19"/>
+    </row>
+    <row r="427" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G427" s="16"/>
+    </row>
+    <row r="428" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G428" s="19"/>
+    </row>
+    <row r="429" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G429" s="16"/>
+    </row>
+    <row r="430" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G430" s="19"/>
+    </row>
+    <row r="431" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G431" s="16"/>
+    </row>
+    <row r="432" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G432" s="19"/>
+    </row>
+    <row r="433" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G433" s="16"/>
+    </row>
+    <row r="434" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G434" s="19"/>
+    </row>
+    <row r="435" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G435" s="16"/>
+    </row>
+    <row r="436" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G436" s="19"/>
+    </row>
+    <row r="437" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G437" s="16"/>
+    </row>
+    <row r="438" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G438" s="19"/>
+    </row>
+    <row r="439" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G439" s="16"/>
+    </row>
+    <row r="440" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G440" s="19"/>
+    </row>
+    <row r="441" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G441" s="16"/>
+    </row>
+    <row r="442" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G442" s="19"/>
+    </row>
+    <row r="443" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G443" s="16"/>
+    </row>
+    <row r="444" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G444" s="19"/>
+    </row>
+    <row r="445" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G445" s="16"/>
+    </row>
+    <row r="446" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G446" s="19"/>
+    </row>
+    <row r="447" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G447" s="16"/>
+    </row>
+    <row r="448" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G448" s="19"/>
+    </row>
+    <row r="449" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G449" s="16"/>
+    </row>
+    <row r="450" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G450" s="19"/>
+    </row>
+    <row r="451" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G451" s="16"/>
+    </row>
+    <row r="452" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G452" s="19"/>
+    </row>
+    <row r="453" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G453" s="16"/>
+    </row>
+    <row r="454" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G454" s="19"/>
+    </row>
+    <row r="455" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G455" s="16"/>
+    </row>
+    <row r="456" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G456" s="19"/>
+    </row>
+    <row r="457" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G457" s="16"/>
+    </row>
+    <row r="458" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G458" s="19"/>
+    </row>
+    <row r="459" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G459" s="16"/>
+    </row>
+    <row r="460" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G460" s="19"/>
+    </row>
+    <row r="461" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G461" s="16"/>
+    </row>
+    <row r="462" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G462" s="19"/>
+    </row>
+    <row r="463" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G463" s="16"/>
+    </row>
+    <row r="464" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G464" s="19"/>
+    </row>
+    <row r="465" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G465" s="16"/>
+    </row>
+    <row r="466" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G466" s="19"/>
+    </row>
+    <row r="467" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G467" s="16"/>
+    </row>
+    <row r="468" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G468" s="19"/>
+    </row>
+    <row r="469" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G469" s="16"/>
+    </row>
+    <row r="470" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G470" s="19"/>
+    </row>
+    <row r="471" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G471" s="16"/>
+    </row>
+    <row r="472" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G472" s="19"/>
+    </row>
+    <row r="473" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G473" s="16"/>
+    </row>
+    <row r="474" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G474" s="19"/>
+    </row>
+    <row r="475" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G475" s="16"/>
+    </row>
+    <row r="476" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G476" s="19"/>
+    </row>
+    <row r="477" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G477" s="16"/>
+    </row>
+    <row r="478" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G478" s="19"/>
+    </row>
+    <row r="479" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G479" s="16"/>
+    </row>
+    <row r="480" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G480" s="19"/>
+    </row>
+    <row r="481" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G481" s="16"/>
+    </row>
+    <row r="482" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G482" s="19"/>
+    </row>
+    <row r="483" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G483" s="16"/>
+    </row>
+    <row r="484" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G484" s="19"/>
+    </row>
+    <row r="485" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G485" s="16"/>
+    </row>
+    <row r="486" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G486" s="19"/>
+    </row>
+    <row r="487" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G487" s="16"/>
+    </row>
+    <row r="488" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G488" s="19"/>
+    </row>
+    <row r="489" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G489" s="16"/>
+    </row>
+    <row r="490" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G490" s="19"/>
+    </row>
+    <row r="491" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G491" s="16"/>
+    </row>
+    <row r="492" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G492" s="19"/>
+    </row>
+    <row r="493" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G493" s="16"/>
+    </row>
+    <row r="494" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G494" s="19"/>
+    </row>
+    <row r="495" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G495" s="16"/>
+    </row>
+    <row r="496" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G496" s="19"/>
+    </row>
+    <row r="497" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G497" s="16"/>
+    </row>
+    <row r="498" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G498" s="19"/>
+    </row>
+    <row r="499" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G499" s="16"/>
+    </row>
+    <row r="500" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G500" s="19"/>
+    </row>
+    <row r="501" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G501" s="16"/>
+    </row>
+    <row r="502" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G502" s="19"/>
+    </row>
+    <row r="503" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G503" s="16"/>
+    </row>
+    <row r="504" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G504" s="19"/>
+    </row>
+    <row r="505" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G505" s="16"/>
+    </row>
+    <row r="506" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G506" s="19"/>
+    </row>
+    <row r="507" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G507" s="16"/>
+    </row>
+    <row r="508" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G508" s="19"/>
+    </row>
+    <row r="509" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G509" s="16"/>
+    </row>
+    <row r="510" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G510" s="19"/>
+    </row>
+    <row r="511" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G511" s="16"/>
+    </row>
+    <row r="512" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G512" s="19"/>
+    </row>
+    <row r="513" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G513" s="16"/>
+    </row>
+    <row r="514" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G514" s="19"/>
+    </row>
+    <row r="515" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G515" s="16"/>
+    </row>
+    <row r="516" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G516" s="19"/>
+    </row>
+    <row r="517" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G517" s="16"/>
+    </row>
+    <row r="518" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G518" s="19"/>
+    </row>
+    <row r="519" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G519" s="16"/>
+    </row>
+    <row r="520" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G520" s="19"/>
+    </row>
+    <row r="521" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G521" s="16"/>
+    </row>
+    <row r="522" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G522" s="19"/>
+    </row>
+    <row r="523" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G523" s="16"/>
+    </row>
+    <row r="524" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G524" s="19"/>
+    </row>
+    <row r="525" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G525" s="16"/>
+    </row>
+    <row r="526" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G526" s="19"/>
+    </row>
+    <row r="527" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G527" s="16"/>
+    </row>
+    <row r="528" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G528" s="19"/>
+    </row>
+    <row r="529" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G529" s="16"/>
+    </row>
+    <row r="530" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G530" s="19"/>
+    </row>
+    <row r="531" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G531" s="16"/>
+    </row>
+    <row r="532" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G532" s="19"/>
+    </row>
+    <row r="533" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G533" s="16"/>
+    </row>
+    <row r="534" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G534" s="19"/>
+    </row>
+    <row r="535" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G535" s="16"/>
+    </row>
+    <row r="536" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G536" s="19"/>
+    </row>
+    <row r="537" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G537" s="16"/>
+    </row>
+    <row r="538" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G538" s="19"/>
+    </row>
+    <row r="539" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G539" s="16"/>
+    </row>
+    <row r="540" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G540" s="19"/>
+    </row>
+    <row r="541" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G541" s="16"/>
+    </row>
+    <row r="542" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G542" s="19"/>
+    </row>
+    <row r="543" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G543" s="16"/>
+    </row>
+    <row r="544" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G544" s="19"/>
+    </row>
+    <row r="545" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G545" s="16"/>
+    </row>
+    <row r="546" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G546" s="19"/>
+    </row>
+    <row r="547" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G547" s="16"/>
+    </row>
+    <row r="548" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G548" s="19"/>
+    </row>
+    <row r="549" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G549" s="16"/>
+    </row>
+    <row r="550" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G550" s="19"/>
+    </row>
+    <row r="551" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G551" s="16"/>
+    </row>
+    <row r="552" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G552" s="19"/>
+    </row>
+    <row r="553" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G553" s="16"/>
+    </row>
+    <row r="554" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G554" s="19"/>
+    </row>
+    <row r="555" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G555" s="16"/>
+    </row>
+    <row r="556" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G556" s="19"/>
+    </row>
+    <row r="557" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G557" s="16"/>
+    </row>
+    <row r="558" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G558" s="19"/>
+    </row>
+    <row r="559" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G559" s="16"/>
+    </row>
+    <row r="560" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G560" s="19"/>
+    </row>
+    <row r="561" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G561" s="16"/>
+    </row>
+    <row r="562" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G562" s="19"/>
+    </row>
+    <row r="563" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G563" s="16"/>
+    </row>
+    <row r="564" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G564" s="19"/>
+    </row>
+    <row r="565" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G565" s="16"/>
+    </row>
+    <row r="566" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G566" s="19"/>
+    </row>
+    <row r="567" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G567" s="16"/>
+    </row>
+    <row r="568" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G568" s="19"/>
+    </row>
+    <row r="569" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G569" s="16"/>
+    </row>
+    <row r="570" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G570" s="19"/>
+    </row>
+    <row r="571" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G571" s="16"/>
+    </row>
+    <row r="572" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G572" s="19"/>
+    </row>
+    <row r="573" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G573" s="16"/>
+    </row>
+    <row r="574" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G574" s="19"/>
+    </row>
+    <row r="575" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G575" s="16"/>
+    </row>
+    <row r="576" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G576" s="19"/>
+    </row>
+    <row r="577" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G577" s="16"/>
+    </row>
+    <row r="578" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G578" s="19"/>
+    </row>
+    <row r="579" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G579" s="16"/>
+    </row>
+    <row r="580" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G580" s="19"/>
+    </row>
+    <row r="581" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G581" s="16"/>
+    </row>
+    <row r="582" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G582" s="19"/>
+    </row>
+    <row r="583" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G583" s="16"/>
+    </row>
+    <row r="584" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G584" s="19"/>
+    </row>
+    <row r="585" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G585" s="16"/>
+    </row>
+    <row r="586" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G586" s="19"/>
+    </row>
+    <row r="587" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G587" s="16"/>
+    </row>
+    <row r="588" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G588" s="19"/>
+    </row>
+    <row r="589" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G589" s="16"/>
+    </row>
+    <row r="590" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G590" s="19"/>
+    </row>
+    <row r="591" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G591" s="16"/>
+    </row>
+    <row r="592" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G592" s="19"/>
+    </row>
+    <row r="593" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G593" s="16"/>
+    </row>
+    <row r="594" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G594" s="19"/>
+    </row>
+    <row r="595" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G595" s="16"/>
+    </row>
+    <row r="596" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G596" s="19"/>
+    </row>
+    <row r="597" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G597" s="16"/>
+    </row>
+    <row r="598" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G598" s="19"/>
+    </row>
+    <row r="599" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G599" s="16"/>
+    </row>
+    <row r="600" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G600" s="19"/>
+    </row>
+    <row r="601" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G601" s="16"/>
+    </row>
+    <row r="602" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G602" s="19"/>
+    </row>
+    <row r="603" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G603" s="16"/>
+    </row>
+    <row r="604" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G604" s="19"/>
+    </row>
+    <row r="605" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G605" s="16"/>
+    </row>
+    <row r="606" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G606" s="19"/>
+    </row>
+    <row r="607" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G607" s="16"/>
+    </row>
+    <row r="608" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G608" s="19"/>
+    </row>
+    <row r="609" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G609" s="16"/>
+    </row>
+    <row r="610" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G610" s="19"/>
+    </row>
+    <row r="611" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G611" s="16"/>
+    </row>
+    <row r="612" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G612" s="19"/>
+    </row>
+    <row r="613" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G613" s="16"/>
+    </row>
+    <row r="614" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G614" s="19"/>
+    </row>
+    <row r="615" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G615" s="16"/>
+    </row>
+    <row r="616" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G616" s="19"/>
+    </row>
+    <row r="617" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G617" s="16"/>
+    </row>
+    <row r="618" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G618" s="19"/>
+    </row>
+    <row r="619" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G619" s="16"/>
+    </row>
+    <row r="620" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G620" s="19"/>
+    </row>
+    <row r="621" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G621" s="16"/>
+    </row>
+    <row r="622" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G622" s="19"/>
+    </row>
+    <row r="623" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G623" s="16"/>
+    </row>
+    <row r="624" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G624" s="19"/>
+    </row>
+    <row r="625" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G625" s="16"/>
+    </row>
+    <row r="626" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G626" s="19"/>
+    </row>
+    <row r="627" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G627" s="16"/>
+    </row>
+    <row r="628" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G628" s="19"/>
+    </row>
+    <row r="629" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G629" s="16"/>
+    </row>
+    <row r="630" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G630" s="19"/>
+    </row>
+    <row r="631" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G631" s="16"/>
+    </row>
+    <row r="632" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G632" s="19"/>
+    </row>
+    <row r="633" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G633" s="16"/>
+    </row>
+    <row r="634" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G634" s="19"/>
+    </row>
+    <row r="635" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G635" s="16"/>
+    </row>
+    <row r="636" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G636" s="19"/>
+    </row>
+    <row r="637" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G637" s="16"/>
+    </row>
+    <row r="638" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G638" s="19"/>
+    </row>
+    <row r="639" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G639" s="16"/>
+    </row>
+    <row r="640" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G640" s="19"/>
+    </row>
+    <row r="641" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G641" s="16"/>
+    </row>
+    <row r="642" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G642" s="19"/>
+    </row>
+    <row r="643" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G643" s="16"/>
+    </row>
+    <row r="644" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G644" s="19"/>
+    </row>
+    <row r="645" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G645" s="16"/>
+    </row>
+    <row r="646" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G646" s="19"/>
+    </row>
+    <row r="647" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G647" s="16"/>
+    </row>
+    <row r="648" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G648" s="19"/>
+    </row>
+    <row r="649" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G649" s="16"/>
+    </row>
+    <row r="650" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G650" s="19"/>
+    </row>
+    <row r="651" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G651" s="16"/>
+    </row>
+    <row r="652" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G652" s="19"/>
+    </row>
+    <row r="653" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G653" s="16"/>
+    </row>
+    <row r="654" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G654" s="19"/>
+    </row>
+    <row r="655" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G655" s="16"/>
+    </row>
+    <row r="656" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G656" s="19"/>
+    </row>
+    <row r="657" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G657" s="16"/>
+    </row>
+    <row r="658" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G658" s="19"/>
+    </row>
+    <row r="659" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G659" s="16"/>
+    </row>
+    <row r="660" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G660" s="19"/>
+    </row>
+    <row r="661" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G661" s="16"/>
+    </row>
+    <row r="662" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G662" s="19"/>
+    </row>
+    <row r="663" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G663" s="16"/>
+    </row>
+    <row r="664" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G664" s="19"/>
+    </row>
+    <row r="665" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G665" s="16"/>
+    </row>
+    <row r="666" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G666" s="19"/>
+    </row>
+    <row r="667" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G667" s="16"/>
+    </row>
+    <row r="668" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G668" s="19"/>
+    </row>
+    <row r="669" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G669" s="16"/>
+    </row>
+    <row r="670" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G670" s="19"/>
+    </row>
+    <row r="671" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G671" s="16"/>
+    </row>
+    <row r="672" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G672" s="19"/>
+    </row>
+    <row r="673" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G673" s="16"/>
+    </row>
+    <row r="674" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G674" s="19"/>
+    </row>
+    <row r="675" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G675" s="16"/>
+    </row>
+    <row r="676" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G676" s="19"/>
+    </row>
+    <row r="677" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G677" s="16"/>
+    </row>
+    <row r="678" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G678" s="19"/>
+    </row>
+    <row r="679" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G679" s="16"/>
+    </row>
+    <row r="680" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G680" s="19"/>
+    </row>
+    <row r="681" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G681" s="16"/>
+    </row>
+    <row r="682" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G682" s="19"/>
+    </row>
+    <row r="683" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G683" s="16"/>
+    </row>
+    <row r="684" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G684" s="19"/>
+    </row>
+    <row r="685" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G685" s="16"/>
+    </row>
+    <row r="686" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G686" s="19"/>
+    </row>
+    <row r="687" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G687" s="16"/>
+    </row>
+    <row r="688" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G688" s="19"/>
+    </row>
+    <row r="689" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G689" s="16"/>
+    </row>
+    <row r="690" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G690" s="19"/>
+    </row>
+    <row r="691" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G691" s="16"/>
+    </row>
+    <row r="692" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G692" s="19"/>
+    </row>
+    <row r="693" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G693" s="16"/>
+    </row>
+    <row r="694" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G694" s="19"/>
+    </row>
+    <row r="695" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G695" s="16"/>
+    </row>
+    <row r="696" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G696" s="19"/>
+    </row>
+    <row r="697" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G697" s="16"/>
+    </row>
+    <row r="698" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G698" s="19"/>
+    </row>
+    <row r="699" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G699" s="16"/>
+    </row>
+    <row r="700" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G700" s="19"/>
+    </row>
+    <row r="701" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G701" s="16"/>
+    </row>
+    <row r="702" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G702" s="19"/>
+    </row>
+    <row r="703" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G703" s="16"/>
+    </row>
+    <row r="704" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G704" s="19"/>
+    </row>
+    <row r="705" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G705" s="16"/>
+    </row>
+    <row r="706" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G706" s="19"/>
+    </row>
+    <row r="707" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G707" s="16"/>
+    </row>
+    <row r="708" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G708" s="19"/>
+    </row>
+    <row r="709" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G709" s="16"/>
+    </row>
+    <row r="710" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G710" s="19"/>
+    </row>
+    <row r="711" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G711" s="16"/>
+    </row>
+    <row r="712" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G712" s="19"/>
+    </row>
+    <row r="713" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G713" s="16"/>
+    </row>
+    <row r="714" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G714" s="19"/>
+    </row>
+    <row r="715" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G715" s="16"/>
+    </row>
+    <row r="716" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G716" s="19"/>
+    </row>
+    <row r="717" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G717" s="16"/>
+    </row>
+    <row r="718" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G718" s="19"/>
+    </row>
+    <row r="719" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G719" s="16"/>
+    </row>
+    <row r="720" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G720" s="19"/>
+    </row>
+    <row r="721" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G721" s="16"/>
+    </row>
+    <row r="722" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G722" s="19"/>
+    </row>
+    <row r="723" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G723" s="16"/>
+    </row>
+    <row r="724" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G724" s="19"/>
+    </row>
+    <row r="725" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G725" s="16"/>
+    </row>
+    <row r="726" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G726" s="19"/>
+    </row>
+    <row r="727" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G727" s="16"/>
+    </row>
+    <row r="728" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G728" s="19"/>
+    </row>
+    <row r="729" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G729" s="16"/>
+    </row>
+    <row r="730" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G730" s="19"/>
+    </row>
+    <row r="731" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G731" s="16"/>
+    </row>
+    <row r="732" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G732" s="19"/>
+    </row>
+    <row r="733" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G733" s="16"/>
+    </row>
+    <row r="734" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G734" s="19"/>
+    </row>
+    <row r="735" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G735" s="16"/>
+    </row>
+    <row r="736" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G736" s="19"/>
+    </row>
+    <row r="737" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G737" s="16"/>
+    </row>
+    <row r="738" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G738" s="19"/>
+    </row>
+    <row r="739" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G739" s="16"/>
+    </row>
+    <row r="740" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G740" s="19"/>
+    </row>
+    <row r="741" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G741" s="16"/>
+    </row>
+    <row r="742" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G742" s="19"/>
+    </row>
+    <row r="743" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G743" s="16"/>
+    </row>
+    <row r="744" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G744" s="19"/>
+    </row>
+    <row r="745" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G745" s="16"/>
+    </row>
+    <row r="746" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G746" s="19"/>
+    </row>
+    <row r="747" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G747" s="16"/>
+    </row>
+    <row r="748" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G748" s="19"/>
+    </row>
+    <row r="749" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G749" s="16"/>
+    </row>
+    <row r="750" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G750" s="19"/>
+    </row>
+    <row r="751" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G751" s="16"/>
+    </row>
+    <row r="752" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G752" s="19"/>
+    </row>
+    <row r="753" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G753" s="16"/>
+    </row>
+    <row r="754" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G754" s="19"/>
+    </row>
+    <row r="755" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G755" s="16"/>
+    </row>
+    <row r="756" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G756" s="19"/>
+    </row>
+    <row r="757" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G757" s="16"/>
+    </row>
+    <row r="758" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G758" s="19"/>
+    </row>
+    <row r="759" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G759" s="16"/>
+    </row>
+    <row r="760" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G760" s="19"/>
+    </row>
+    <row r="761" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G761" s="16"/>
+    </row>
+    <row r="762" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G762" s="19"/>
+    </row>
+    <row r="763" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G763" s="16"/>
+    </row>
+    <row r="764" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G764" s="19"/>
+    </row>
+    <row r="765" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G765" s="16"/>
+    </row>
+    <row r="766" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G766" s="19"/>
+    </row>
+    <row r="767" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G767" s="16"/>
+    </row>
+    <row r="768" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G768" s="19"/>
+    </row>
+    <row r="769" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G769" s="16"/>
+    </row>
+    <row r="770" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G770" s="19"/>
+    </row>
+    <row r="771" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G771" s="16"/>
+    </row>
+    <row r="772" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G772" s="19"/>
+    </row>
+    <row r="773" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G773" s="16"/>
+    </row>
+    <row r="774" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G774" s="19"/>
+    </row>
+    <row r="775" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G775" s="16"/>
+    </row>
+    <row r="776" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G776" s="19"/>
+    </row>
+    <row r="777" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G777" s="16"/>
+    </row>
+    <row r="778" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G778" s="19"/>
+    </row>
+    <row r="779" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G779" s="16"/>
+    </row>
+    <row r="780" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G780" s="19"/>
+    </row>
+    <row r="781" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G781" s="16"/>
+    </row>
+    <row r="782" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G782" s="19"/>
+    </row>
+    <row r="783" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G783" s="16"/>
+    </row>
+    <row r="784" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G784" s="19"/>
+    </row>
+    <row r="785" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G785" s="16"/>
+    </row>
+    <row r="786" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G786" s="19"/>
+    </row>
+    <row r="787" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G787" s="16"/>
+    </row>
+    <row r="788" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G788" s="19"/>
+    </row>
+    <row r="789" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G789" s="16"/>
+    </row>
+    <row r="790" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G790" s="19"/>
+    </row>
+    <row r="791" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G791" s="16"/>
+    </row>
+    <row r="792" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G792" s="19"/>
+    </row>
+    <row r="793" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G793" s="16"/>
+    </row>
+    <row r="794" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G794" s="19"/>
+    </row>
+    <row r="795" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G795" s="16"/>
+    </row>
+    <row r="796" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G796" s="19"/>
+    </row>
+    <row r="797" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G797" s="16"/>
+    </row>
+    <row r="798" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G798" s="19"/>
+    </row>
+    <row r="799" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G799" s="16"/>
+    </row>
+    <row r="800" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G800" s="19"/>
+    </row>
+    <row r="801" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G801" s="16"/>
+    </row>
+    <row r="802" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G802" s="19"/>
+    </row>
+    <row r="803" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G803" s="16"/>
+    </row>
+    <row r="804" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G804" s="19"/>
+    </row>
+    <row r="805" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G805" s="16"/>
+    </row>
+    <row r="806" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G806" s="19"/>
+    </row>
+    <row r="807" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G807" s="16"/>
+    </row>
+    <row r="808" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G808" s="19"/>
+    </row>
+    <row r="809" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G809" s="16"/>
+    </row>
+    <row r="810" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G810" s="19"/>
+    </row>
+    <row r="811" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G811" s="16"/>
+    </row>
+    <row r="812" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G812" s="19"/>
+    </row>
+    <row r="813" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G813" s="16"/>
+    </row>
+    <row r="814" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G814" s="19"/>
+    </row>
+    <row r="815" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G815" s="16"/>
+    </row>
+    <row r="816" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G816" s="19"/>
+    </row>
+    <row r="817" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G817" s="16"/>
+    </row>
+    <row r="818" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G818" s="19"/>
+    </row>
+    <row r="819" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G819" s="16"/>
+    </row>
+    <row r="820" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G820" s="19"/>
+    </row>
+    <row r="821" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G821" s="16"/>
+    </row>
+    <row r="822" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G822" s="19"/>
+    </row>
+    <row r="823" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G823" s="16"/>
+    </row>
+    <row r="824" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G824" s="19"/>
+    </row>
+    <row r="825" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G825" s="16"/>
+    </row>
+    <row r="826" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G826" s="19"/>
+    </row>
+    <row r="827" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G827" s="16"/>
+    </row>
+    <row r="828" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G828" s="19"/>
+    </row>
+    <row r="829" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G829" s="16"/>
+    </row>
+    <row r="830" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G830" s="19"/>
+    </row>
+    <row r="831" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G831" s="16"/>
+    </row>
+    <row r="832" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G832" s="19"/>
+    </row>
+    <row r="833" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G833" s="16"/>
+    </row>
+    <row r="834" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G834" s="19"/>
+    </row>
+    <row r="835" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G835" s="16"/>
+    </row>
+    <row r="836" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G836" s="19"/>
+    </row>
+    <row r="837" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G837" s="16"/>
+    </row>
+    <row r="838" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G838" s="19"/>
+    </row>
+    <row r="839" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G839" s="16"/>
+    </row>
+    <row r="840" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G840" s="19"/>
+    </row>
+    <row r="841" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G841" s="16"/>
+    </row>
+    <row r="842" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G842" s="19"/>
+    </row>
+    <row r="843" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G843" s="16"/>
+    </row>
+    <row r="844" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G844" s="19"/>
+    </row>
+    <row r="845" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G845" s="16"/>
+    </row>
+    <row r="846" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G846" s="19"/>
+    </row>
+    <row r="847" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G847" s="16"/>
+    </row>
+    <row r="848" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G848" s="19"/>
+    </row>
+    <row r="849" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G849" s="16"/>
+    </row>
+    <row r="850" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G850" s="19"/>
+    </row>
+    <row r="851" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G851" s="16"/>
+    </row>
+    <row r="852" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G852" s="19"/>
+    </row>
+    <row r="853" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G853" s="16"/>
+    </row>
+    <row r="854" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G854" s="19"/>
+    </row>
+    <row r="855" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G855" s="16"/>
+    </row>
+    <row r="856" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G856" s="19"/>
+    </row>
+    <row r="857" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G857" s="16"/>
+    </row>
+    <row r="858" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G858" s="19"/>
+    </row>
+    <row r="859" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G859" s="16"/>
+    </row>
+    <row r="860" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G860" s="19"/>
+    </row>
+    <row r="861" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G861" s="16"/>
+    </row>
+    <row r="862" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G862" s="19"/>
+    </row>
+    <row r="863" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G863" s="16"/>
+    </row>
+    <row r="864" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G864" s="19"/>
+    </row>
+    <row r="865" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G865" s="16"/>
+    </row>
+    <row r="866" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G866" s="19"/>
+    </row>
+    <row r="867" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G867" s="16"/>
+    </row>
+    <row r="868" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G868" s="19"/>
+    </row>
+    <row r="869" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G869" s="16"/>
+    </row>
+    <row r="870" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G870" s="19"/>
+    </row>
+    <row r="871" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G871" s="16"/>
+    </row>
+    <row r="872" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G872" s="19"/>
+    </row>
+    <row r="873" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G873" s="16"/>
+    </row>
+    <row r="874" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G874" s="19"/>
+    </row>
+    <row r="875" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G875" s="16"/>
+    </row>
+    <row r="876" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G876" s="19"/>
+    </row>
+    <row r="877" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G877" s="16"/>
+    </row>
+    <row r="878" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G878" s="19"/>
+    </row>
+    <row r="879" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G879" s="16"/>
+    </row>
+    <row r="880" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G880" s="19"/>
+    </row>
+    <row r="881" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G881" s="16"/>
+    </row>
+    <row r="882" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G882" s="19"/>
+    </row>
+    <row r="883" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G883" s="16"/>
+    </row>
+    <row r="884" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G884" s="19"/>
+    </row>
+    <row r="885" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G885" s="16"/>
+    </row>
+    <row r="886" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G886" s="19"/>
+    </row>
+    <row r="887" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G887" s="16"/>
+    </row>
+    <row r="888" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G888" s="19"/>
+    </row>
+    <row r="889" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G889" s="16"/>
+    </row>
+    <row r="890" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G890" s="19"/>
+    </row>
+    <row r="891" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G891" s="16"/>
+    </row>
+    <row r="892" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G892" s="19"/>
+    </row>
+    <row r="893" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G893" s="16"/>
+    </row>
+    <row r="894" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G894" s="19"/>
+    </row>
+    <row r="895" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G895" s="16"/>
+    </row>
+    <row r="896" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G896" s="19"/>
+    </row>
+    <row r="897" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G897" s="16"/>
+    </row>
+    <row r="898" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G898" s="19"/>
+    </row>
+    <row r="899" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G899" s="16"/>
+    </row>
+    <row r="900" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G900" s="19"/>
+    </row>
+    <row r="901" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G901" s="16"/>
+    </row>
+    <row r="902" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G902" s="19"/>
+    </row>
+    <row r="903" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G903" s="16"/>
+    </row>
+    <row r="904" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G904" s="19"/>
+    </row>
+    <row r="905" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G905" s="16"/>
+    </row>
+    <row r="906" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G906" s="19"/>
+    </row>
+    <row r="907" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G907" s="16"/>
+    </row>
+    <row r="908" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G908" s="19"/>
+    </row>
+    <row r="909" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G909" s="16"/>
+    </row>
+    <row r="910" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G910" s="19"/>
+    </row>
+    <row r="911" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G911" s="16"/>
+    </row>
+    <row r="912" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G912" s="19"/>
+    </row>
+    <row r="913" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G913" s="16"/>
+    </row>
+    <row r="914" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G914" s="19"/>
+    </row>
+    <row r="915" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G915" s="16"/>
+    </row>
+    <row r="916" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G916" s="19"/>
+    </row>
+    <row r="917" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G917" s="16"/>
+    </row>
+    <row r="918" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G918" s="19"/>
+    </row>
+    <row r="919" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G919" s="16"/>
+    </row>
+    <row r="920" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G920" s="19"/>
+    </row>
+    <row r="921" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G921" s="16"/>
+    </row>
+    <row r="922" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G922" s="19"/>
+    </row>
+    <row r="923" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G923" s="16"/>
+    </row>
+    <row r="924" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G924" s="19"/>
+    </row>
+    <row r="925" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G925" s="16"/>
+    </row>
+    <row r="926" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G926" s="19"/>
+    </row>
+    <row r="927" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G927" s="16"/>
+    </row>
+    <row r="928" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G928" s="19"/>
+    </row>
+    <row r="929" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G929" s="16"/>
+    </row>
+    <row r="930" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G930" s="19"/>
+    </row>
+    <row r="931" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G931" s="16"/>
+    </row>
+    <row r="932" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G932" s="19"/>
+    </row>
+    <row r="933" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G933" s="16"/>
+    </row>
+    <row r="934" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G934" s="19"/>
+    </row>
+    <row r="935" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G935" s="16"/>
+    </row>
+    <row r="936" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G936" s="19"/>
+    </row>
+    <row r="937" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G937" s="16"/>
+    </row>
+    <row r="938" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G938" s="19"/>
+    </row>
+    <row r="939" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G939" s="16"/>
+    </row>
+    <row r="940" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G940" s="19"/>
+    </row>
+    <row r="941" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G941" s="16"/>
+    </row>
+    <row r="942" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G942" s="19"/>
+    </row>
+    <row r="943" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G943" s="16"/>
+    </row>
+    <row r="944" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G944" s="19"/>
+    </row>
+    <row r="945" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G945" s="16"/>
+    </row>
+    <row r="946" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G946" s="19"/>
+    </row>
+    <row r="947" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G947" s="16"/>
+    </row>
+    <row r="948" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G948" s="19"/>
+    </row>
+    <row r="949" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G949" s="16"/>
+    </row>
+    <row r="950" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G950" s="19"/>
+    </row>
+    <row r="951" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G951" s="16"/>
+    </row>
+    <row r="952" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G952" s="19"/>
+    </row>
+    <row r="953" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G953" s="16"/>
+    </row>
+    <row r="954" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G954" s="19"/>
+    </row>
+    <row r="955" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G955" s="16"/>
+    </row>
+    <row r="956" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G956" s="19"/>
+    </row>
+    <row r="957" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G957" s="16"/>
+    </row>
+    <row r="958" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G958" s="19"/>
+    </row>
+    <row r="959" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G959" s="16"/>
+    </row>
+    <row r="960" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G960" s="19"/>
+    </row>
+    <row r="961" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G961" s="16"/>
+    </row>
+    <row r="962" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G962" s="19"/>
+    </row>
+    <row r="963" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G963" s="16"/>
+    </row>
+    <row r="964" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G964" s="19"/>
+    </row>
+    <row r="965" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G965" s="16"/>
+    </row>
+    <row r="966" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G966" s="19"/>
+    </row>
+    <row r="967" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G967" s="16"/>
+    </row>
+    <row r="968" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G968" s="19"/>
+    </row>
+    <row r="969" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G969" s="16"/>
+    </row>
+    <row r="970" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G970" s="19"/>
+    </row>
+    <row r="971" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G971" s="16"/>
+    </row>
+    <row r="972" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G972" s="19"/>
+    </row>
+    <row r="973" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G973" s="16"/>
+    </row>
+    <row r="974" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G974" s="19"/>
+    </row>
+    <row r="975" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G975" s="16"/>
+    </row>
+    <row r="976" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G976" s="19"/>
+    </row>
+    <row r="977" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G977" s="16"/>
+    </row>
+    <row r="978" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G978" s="19"/>
+    </row>
+    <row r="979" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G979" s="16"/>
+    </row>
+    <row r="980" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G980" s="19"/>
+    </row>
+    <row r="981" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G981" s="16"/>
+    </row>
+    <row r="982" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G982" s="19"/>
+    </row>
+    <row r="983" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G983" s="16"/>
+    </row>
+    <row r="984" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G984" s="19"/>
+    </row>
+    <row r="985" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G985" s="16"/>
+    </row>
+    <row r="986" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G986" s="19"/>
+    </row>
+    <row r="987" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G987" s="16"/>
+    </row>
+    <row r="988" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G988" s="19"/>
+    </row>
+    <row r="989" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G989" s="16"/>
+    </row>
+    <row r="990" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G990" s="37"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:O39" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Correcting the Data Dictionary Asset
Linking the right Data Dictionary
</commit_message>
<xml_diff>
--- a/assets/data/CCLF_BCDA_BB_Crosswalk.xlsx
+++ b/assets/data/CCLF_BCDA_BB_Crosswalk.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesmcconnell/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A22E19FD-EF4E-AB44-8C2A-DCF39AE31980}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA1AC24-1899-D242-B062-B17E64EA89E9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="860" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2444" uniqueCount="871">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2445" uniqueCount="872">
   <si>
     <t>CCLF Claim Field Label</t>
   </si>
@@ -2986,9 +2986,6 @@
     <t>Patient.address.state</t>
   </si>
   <si>
-    <t>Patient.address.district</t>
-  </si>
-  <si>
     <t>Patient.address.postalCode</t>
   </si>
   <si>
@@ -3176,6 +3173,12 @@
   <si>
     <t xml:space="preserve">ExplanationOfBenefit.identifier.value
  </t>
+  </si>
+  <si>
+    <t>No longer Mapped, use Beneficiary mailing addresses to get county information</t>
+  </si>
+  <si>
+    <t>Not Mapped, use Beneficiary DOB to calculate age</t>
   </si>
 </sst>
 </file>
@@ -3256,7 +3259,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3353,6 +3356,12 @@
         <bgColor rgb="FFD9D9D9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -3366,7 +3375,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -3571,6 +3580,21 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4131,18 +4155,18 @@
   <dimension ref="A1:R990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E186" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F25" sqref="F25"/>
+      <selection pane="bottomRight" activeCell="G195" sqref="G195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="29.5" style="7" customWidth="1"/>
     <col min="2" max="2" width="24.83203125" customWidth="1"/>
-    <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="45" customWidth="1"/>
     <col min="6" max="6" width="82.6640625" style="34" customWidth="1"/>
     <col min="7" max="7" width="64.5" customWidth="1"/>
@@ -5401,7 +5425,7 @@
         <v>208</v>
       </c>
       <c r="F25" s="40" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="G25" s="41"/>
       <c r="H25" s="39" t="s">
@@ -5447,7 +5471,7 @@
         <v>211</v>
       </c>
       <c r="F26" s="37" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="G26" s="21"/>
       <c r="H26" s="3" t="s">
@@ -5899,7 +5923,7 @@
         <v>728</v>
       </c>
       <c r="F35" s="40" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="G35" s="41"/>
       <c r="H35" s="39" t="s">
@@ -5999,7 +6023,7 @@
         <v>731</v>
       </c>
       <c r="F37" s="40" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="G37" s="41"/>
       <c r="H37" s="39" t="s">
@@ -6049,7 +6073,7 @@
         <v>732</v>
       </c>
       <c r="F38" s="46" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="G38" s="47"/>
       <c r="H38" s="45" t="s">
@@ -6521,7 +6545,7 @@
         <v>78</v>
       </c>
       <c r="F48" s="46" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="G48" s="47"/>
       <c r="H48" s="45" t="s">
@@ -7240,7 +7264,7 @@
         <v>751</v>
       </c>
       <c r="G63" s="50" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H63" s="1" t="s">
         <v>449</v>
@@ -9437,7 +9461,7 @@
         <v>357</v>
       </c>
       <c r="F108" s="46" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="G108" s="47"/>
       <c r="H108" s="45" t="s">
@@ -9687,7 +9711,7 @@
         <v>375</v>
       </c>
       <c r="F113" s="40" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="G113" s="41"/>
       <c r="H113" s="39" t="s">
@@ -9733,7 +9757,7 @@
         <v>211</v>
       </c>
       <c r="F114" s="37" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="G114" s="21"/>
       <c r="H114" s="3" t="s">
@@ -11956,7 +11980,7 @@
         <v>463</v>
       </c>
       <c r="F159" s="40" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="G159" s="41"/>
       <c r="H159" s="39" t="s">
@@ -12046,7 +12070,7 @@
         <v>464</v>
       </c>
       <c r="F161" s="17" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="G161" s="18"/>
       <c r="H161" s="1" t="s">
@@ -12622,7 +12646,7 @@
         <v>484</v>
       </c>
       <c r="F173" s="59" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="G173" s="41"/>
       <c r="H173" s="39" t="s">
@@ -12672,7 +12696,7 @@
         <v>490</v>
       </c>
       <c r="F174" s="14" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="G174" s="15"/>
       <c r="H174" s="2" t="s">
@@ -13072,7 +13096,7 @@
         <v>522</v>
       </c>
       <c r="F182" s="63" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="G182" s="64"/>
       <c r="H182" s="62" t="s">
@@ -13118,7 +13142,7 @@
         <v>523</v>
       </c>
       <c r="F183" s="37" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="G183" s="21"/>
       <c r="H183" s="3" t="s">
@@ -13461,51 +13485,51 @@
       <c r="Q190" s="5"/>
       <c r="R190" s="2"/>
     </row>
-    <row r="191" spans="1:18" ht="30">
-      <c r="A191" s="4" t="s">
+    <row r="191" spans="1:18" s="60" customFormat="1" ht="30">
+      <c r="A191" s="73" t="s">
         <v>544</v>
       </c>
-      <c r="B191" s="1" t="s">
+      <c r="B191" s="74" t="s">
         <v>545</v>
       </c>
-      <c r="C191" s="1"/>
-      <c r="D191" s="1"/>
-      <c r="E191" s="1" t="s">
+      <c r="C191" s="74"/>
+      <c r="D191" s="74"/>
+      <c r="E191" s="74" t="s">
         <v>546</v>
       </c>
-      <c r="F191" s="17" t="s">
-        <v>826</v>
-      </c>
-      <c r="G191" s="18"/>
-      <c r="H191" s="1" t="s">
+      <c r="F191" s="75"/>
+      <c r="G191" s="76" t="s">
+        <v>870</v>
+      </c>
+      <c r="H191" s="74" t="s">
         <v>540</v>
       </c>
-      <c r="I191" s="1">
+      <c r="I191" s="74">
         <v>4</v>
       </c>
-      <c r="J191" s="19" t="s">
+      <c r="J191" s="77" t="s">
         <v>42</v>
       </c>
-      <c r="K191" s="1">
+      <c r="K191" s="74">
         <v>25</v>
       </c>
-      <c r="L191" s="1">
+      <c r="L191" s="74">
         <v>27</v>
       </c>
-      <c r="M191" s="1">
+      <c r="M191" s="74">
         <v>3</v>
       </c>
-      <c r="N191" s="1" t="s">
+      <c r="N191" s="74" t="s">
         <v>547</v>
       </c>
-      <c r="O191" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="P191" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q191" s="4"/>
-      <c r="R191" s="1"/>
+      <c r="O191" s="74" t="s">
+        <v>20</v>
+      </c>
+      <c r="P191" s="74" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q191" s="73"/>
+      <c r="R191" s="74"/>
     </row>
     <row r="192" spans="1:18" ht="30">
       <c r="A192" s="5" t="s">
@@ -13520,7 +13544,7 @@
         <v>550</v>
       </c>
       <c r="F192" s="14" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="G192" s="15"/>
       <c r="H192" s="2" t="s">
@@ -13612,7 +13636,7 @@
         <v>557</v>
       </c>
       <c r="F194" s="14" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="G194" s="15"/>
       <c r="H194" s="2" t="s">
@@ -13644,7 +13668,7 @@
       </c>
       <c r="Q194" s="5"/>
       <c r="R194" s="2" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="195" spans="1:18" ht="120">
@@ -13660,7 +13684,7 @@
         <v>560</v>
       </c>
       <c r="F195" s="17" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="G195" s="18"/>
       <c r="H195" s="1" t="s">
@@ -13692,7 +13716,7 @@
       </c>
       <c r="Q195" s="4"/>
       <c r="R195" s="1" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="196" spans="1:18" s="60" customFormat="1" ht="45">
@@ -13708,7 +13732,9 @@
         <v>563</v>
       </c>
       <c r="F196" s="37"/>
-      <c r="G196" s="68"/>
+      <c r="G196" s="68" t="s">
+        <v>871</v>
+      </c>
       <c r="H196" s="67" t="s">
         <v>540</v>
       </c>
@@ -13749,16 +13775,16 @@
         <v>565</v>
       </c>
       <c r="C197" s="1" t="s">
+        <v>831</v>
+      </c>
+      <c r="D197" s="1" t="s">
         <v>832</v>
-      </c>
-      <c r="D197" s="1" t="s">
-        <v>833</v>
       </c>
       <c r="E197" s="1" t="s">
         <v>566</v>
       </c>
       <c r="F197" s="17" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="G197" s="18"/>
       <c r="H197" s="1" t="s">
@@ -13806,7 +13832,7 @@
         <v>569</v>
       </c>
       <c r="F198" s="36" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="G198" s="15"/>
       <c r="H198" s="2" t="s">
@@ -13837,7 +13863,7 @@
         <v>20</v>
       </c>
       <c r="Q198" s="5" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="R198" s="2" t="s">
         <v>667</v>
@@ -13858,7 +13884,7 @@
         <v>572</v>
       </c>
       <c r="F199" s="40" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="G199" s="41"/>
       <c r="H199" s="39" t="s">
@@ -13904,7 +13930,7 @@
         <v>575</v>
       </c>
       <c r="F200" s="63" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="G200" s="64"/>
       <c r="H200" s="62" t="s">
@@ -13950,7 +13976,7 @@
         <v>578</v>
       </c>
       <c r="F201" s="40" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="G201" s="41"/>
       <c r="H201" s="39" t="s">
@@ -13996,7 +14022,7 @@
         <v>581</v>
       </c>
       <c r="F202" s="14" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="G202" s="15"/>
       <c r="H202" s="2" t="s">
@@ -14042,7 +14068,7 @@
         <v>585</v>
       </c>
       <c r="F203" s="17" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="G203" s="18"/>
       <c r="H203" s="1" t="s">
@@ -14088,7 +14114,7 @@
         <v>588</v>
       </c>
       <c r="F204" s="14" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="G204" s="15"/>
       <c r="H204" s="2" t="s">
@@ -14134,7 +14160,7 @@
         <v>591</v>
       </c>
       <c r="F205" s="17" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="G205" s="18"/>
       <c r="H205" s="1" t="s">
@@ -14182,7 +14208,7 @@
         <v>594</v>
       </c>
       <c r="F206" s="14" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="G206" s="15"/>
       <c r="H206" s="2" t="s">
@@ -14213,7 +14239,7 @@
         <v>20</v>
       </c>
       <c r="Q206" s="5" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="R206" s="2" t="s">
         <v>669</v>
@@ -14232,7 +14258,7 @@
         <v>597</v>
       </c>
       <c r="F207" s="17" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="G207" s="18"/>
       <c r="H207" s="1" t="s">
@@ -14278,7 +14304,7 @@
         <v>600</v>
       </c>
       <c r="F208" s="14" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="G208" s="15"/>
       <c r="H208" s="2" t="s">
@@ -14324,7 +14350,7 @@
         <v>603</v>
       </c>
       <c r="F209" s="40" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="G209" s="41"/>
       <c r="H209" s="39" t="s">
@@ -14370,7 +14396,7 @@
         <v>607</v>
       </c>
       <c r="F210" s="63" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="G210" s="64"/>
       <c r="H210" s="62" t="s">
@@ -14416,7 +14442,7 @@
         <v>610</v>
       </c>
       <c r="F211" s="40" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="G211" s="41"/>
       <c r="H211" s="39" t="s">
@@ -14462,7 +14488,7 @@
         <v>613</v>
       </c>
       <c r="F212" s="63" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="G212" s="64"/>
       <c r="H212" s="62" t="s">
@@ -14508,7 +14534,7 @@
         <v>616</v>
       </c>
       <c r="F213" s="40" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="G213" s="41"/>
       <c r="H213" s="39" t="s">
@@ -14554,7 +14580,7 @@
         <v>619</v>
       </c>
       <c r="F214" s="63" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="G214" s="64"/>
       <c r="H214" s="62" t="s">
@@ -14692,7 +14718,7 @@
         <v>629</v>
       </c>
       <c r="F217" s="17" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="G217" s="18"/>
       <c r="H217" s="1" t="s">
@@ -14738,7 +14764,7 @@
         <v>632</v>
       </c>
       <c r="F218" s="14" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="G218" s="15"/>
       <c r="H218" s="2" t="s">
@@ -14804,7 +14830,7 @@
         <v>637</v>
       </c>
       <c r="F220" s="14" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="G220" s="15"/>
       <c r="H220" s="2" t="s">
@@ -14852,7 +14878,7 @@
         <v>642</v>
       </c>
       <c r="F221" s="17" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="G221" s="18"/>
       <c r="H221" s="1" t="s">
@@ -14898,7 +14924,7 @@
         <v>645</v>
       </c>
       <c r="F222" s="14" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="G222" s="15"/>
       <c r="H222" s="2" t="s">
@@ -14940,13 +14966,13 @@
       </c>
       <c r="C223" s="39"/>
       <c r="D223" s="39" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="E223" s="39" t="s">
         <v>648</v>
       </c>
       <c r="F223" s="40" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="G223" s="41"/>
       <c r="H223" s="39" t="s">
@@ -14988,13 +15014,13 @@
       </c>
       <c r="C224" s="62"/>
       <c r="D224" s="62" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="E224" s="62" t="s">
         <v>651</v>
       </c>
       <c r="F224" s="63" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="G224" s="64"/>
       <c r="H224" s="62" t="s">
@@ -15037,10 +15063,10 @@
       <c r="C225" s="1"/>
       <c r="D225" s="1"/>
       <c r="E225" s="1" t="s">
+        <v>847</v>
+      </c>
+      <c r="F225" s="17" t="s">
         <v>848</v>
-      </c>
-      <c r="F225" s="17" t="s">
-        <v>849</v>
       </c>
       <c r="G225" s="18"/>
       <c r="H225" s="1" t="s">
@@ -15109,7 +15135,7 @@
         <v>683</v>
       </c>
       <c r="G227" s="50" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H227" s="10" t="s">
         <v>671</v>
@@ -15250,7 +15276,7 @@
         <v>674</v>
       </c>
       <c r="F230" s="14" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="G230" s="15"/>
       <c r="H230" s="9" t="s">
@@ -15298,7 +15324,7 @@
         <v>677</v>
       </c>
       <c r="F231" s="17" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="G231" s="17"/>
       <c r="H231" s="10" t="s">
@@ -15554,7 +15580,7 @@
         <v>679</v>
       </c>
       <c r="F237" s="17" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="G237" s="18"/>
       <c r="H237" s="10" t="s">

</xml_diff>